<commit_message>
Controlador PID - Previo Terminado
</commit_message>
<xml_diff>
--- a/4. CONTROLADOR PID/INFORME PREVIO/calculo_rc.xlsx
+++ b/4. CONTROLADOR PID/INFORME PREVIO/calculo_rc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\lab-control-i\4. CONTROLADOR PID\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9D2EAF-DF72-488F-A791-D25DC1909504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0AE6A8-0830-4B6A-BB2D-00574307F44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="13935" windowHeight="16200" activeTab="1" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
   <si>
     <t>R</t>
   </si>
@@ -112,16 +112,13 @@
     <t>Salida Mp Final</t>
   </si>
   <si>
-    <t>Sobr Amortiguado</t>
-  </si>
-  <si>
-    <t>Sub Amortiguado</t>
-  </si>
-  <si>
-    <t>Sub Amortiguado PID</t>
-  </si>
-  <si>
-    <t>Sobre Amortiguado PID</t>
+    <t>SubAmortiguado</t>
+  </si>
+  <si>
+    <t>Te/2</t>
+  </si>
+  <si>
+    <t>Ts/2</t>
   </si>
 </sst>
 </file>
@@ -495,17 +492,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815D4429-F3D6-4F7B-A018-34B483DED09C}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -515,7 +512,7 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="F1" s="4" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -578,11 +575,11 @@
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C10" si="0">3/(2*$D$2*B4)</f>
-        <v>7500.0000000000009</v>
+        <f>3/($D$2*B4)</f>
+        <v>15000.000000000002</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F11" si="1">($G$2^2*4*G4)/9</f>
+        <f>($G$2^2*4*G4)/9</f>
         <v>4.4469653998865575E-6</v>
       </c>
       <c r="G4">
@@ -590,8 +587,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="H4">
-        <f>3/(2*$I$2*G4)</f>
-        <v>3571.4285714285716</v>
+        <f>3/($I$2*G4)</f>
+        <v>7142.8571428571431</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -604,11 +601,11 @@
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>1595.7446808510638</v>
+        <f t="shared" ref="C5:C16" si="0">3/($D$2*B5)</f>
+        <v>3191.4893617021276</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F5:F10" si="1">($G$2^2*4*G5)/9</f>
         <v>2.0900737379466819E-5</v>
       </c>
       <c r="G5">
@@ -616,22 +613,22 @@
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H12" si="2">3/(2*$I$2*G5)</f>
-        <v>759.87841945288756</v>
+        <f t="shared" ref="H5:H10" si="2">3/($I$2*G5)</f>
+        <v>1519.7568389057751</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <f>$B$2^2*4*B6/(9)</f>
         <v>1.3675213675213674E-5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>750</v>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
@@ -643,7 +640,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>357.14285714285717</v>
+        <v>714.28571428571433</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -657,7 +654,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>159.57446808510639</v>
+        <v>319.14893617021278</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
@@ -669,7 +666,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>75.98784194528875</v>
+        <v>151.9756838905775</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -683,7 +680,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
@@ -695,7 +692,7 @@
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>35.714285714285715</v>
+        <v>71.428571428571431</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -709,19 +706,19 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>3409.0909090909095</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
+        <v>6818.1818181818189</v>
+      </c>
+      <c r="F9" s="1">
+        <f>($G$2^2*4*G9)/9</f>
         <v>9.7833238797504279E-6</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <f t="shared" si="2"/>
-        <v>1623.3766233766235</v>
+        <v>3246.7532467532469</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -735,7 +732,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
@@ -747,7 +744,7 @@
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>7598.7841945288756</v>
+        <v>15197.568389057751</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -760,16 +757,8 @@
         <v>1E-3</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C16" si="5">3/(2*$D$2*B11)</f>
-        <v>75</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H11" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,12 +771,8 @@
         <v>1E-3</v>
       </c>
       <c r="C12">
-        <f t="shared" si="5"/>
-        <v>75</v>
-      </c>
-      <c r="H12" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -800,8 +785,8 @@
         <v>1E-3</v>
       </c>
       <c r="C13">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -814,8 +799,8 @@
         <v>1E-3</v>
       </c>
       <c r="C14">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -828,8 +813,8 @@
         <v>1E-3</v>
       </c>
       <c r="C15">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -842,8 +827,8 @@
         <v>1E-3</v>
       </c>
       <c r="C16">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -922,8 +907,11 @@
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -936,6 +924,10 @@
       <c r="F28">
         <f>F26*4</f>
         <v>0.38116846284741923</v>
+      </c>
+      <c r="G28">
+        <f>F28/2</f>
+        <v>0.19058423142370962</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1034,115 +1026,38 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="F41" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>325</v>
-      </c>
-      <c r="B44">
-        <f>SQRT(A44)</f>
-        <v>18.027756377319946</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <f>D17/(2*B44)</f>
-        <v>0</v>
-      </c>
+      <c r="B45" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <f>PI()/(B48)</f>
-        <v>0.17426420614059965</v>
-      </c>
-      <c r="B48" s="3">
-        <f>B44*SQRT(1-B46^2)</f>
-        <v>18.027756377319946</v>
-      </c>
+      <c r="B48" s="3"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="e">
-        <f>4/(B46*B44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B50">
-        <f>1.8/(B44)</f>
-        <v>9.9846035320541246E-2</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <f>B44*B46</f>
-        <v>0</v>
-      </c>
-      <c r="B52">
-        <v>12.361000000000001</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <f>1+1*B52%</f>
-        <v>1.12361</v>
-      </c>
-      <c r="B54">
-        <f>1+(B52%/2)</f>
-        <v>1.0618050000000001</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1159,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03516E6C-2C46-4AD1-BC3F-907E935C7AD3}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,8 +1142,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="C3">
-        <f>3/(2*$D$1*B3)</f>
-        <v>75000</v>
+        <f>3/($D$1*B3)</f>
+        <v>150000</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G10" si="0">($H$1^2*4*H3)/9</f>
@@ -1239,228 +1154,304 @@
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="I3">
-        <f>3/(2*$J$1*H3)</f>
-        <v>4838.709677419356</v>
+        <f>3/($J$1*H3)</f>
+        <v>9677.419354838712</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>$B$1^2*4*B4/(9)</f>
-        <v>6.8376068376068378E-7</v>
+        <v>1.5042735042735044E-7</v>
       </c>
       <c r="B4">
-        <f>100*10^-6</f>
-        <v>9.9999999999999991E-5</v>
+        <f>22*10^-6</f>
+        <v>2.1999999999999999E-5</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C15" si="1">3/(2*$D$1*B4)</f>
-        <v>7500.0000000000009</v>
+        <f t="shared" ref="C4:C15" si="1">3/($D$1*B4)</f>
+        <v>68181.818181818177</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>4.9606400825913007E-5</v>
+        <v>1.0913408181700861E-5</v>
       </c>
       <c r="H4">
-        <f>100*10^-6</f>
-        <v>9.9999999999999991E-5</v>
+        <f>22*10^-6</f>
+        <v>2.1999999999999999E-5</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I11" si="2">3/(2*$J$1*H4)</f>
-        <v>483.87096774193549</v>
+        <f t="shared" ref="I4:I15" si="2">3/($J$1*H4)</f>
+        <v>4398.8269794721409</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>$B$1^2*4*B5/(9)</f>
-        <v>3.213675213675214E-6</v>
+        <v>3.2136752136752138E-7</v>
       </c>
       <c r="B5">
-        <f>470*10^-6</f>
-        <v>4.6999999999999999E-4</v>
+        <f>47*10^-6</f>
+        <v>4.6999999999999997E-5</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>1595.7446808510638</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>2.3315008388179114E-4</v>
-      </c>
-      <c r="H5">
-        <f>470*10^-6</f>
-        <v>4.6999999999999999E-4</v>
-      </c>
-      <c r="I5">
+        <v>31914.89361702128</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3315008388179114E-5</v>
+      </c>
+      <c r="H5" s="1">
+        <f>47*10^-6</f>
+        <v>4.6999999999999997E-5</v>
+      </c>
+      <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>102.95126973232671</v>
+        <v>2059.0253946465341</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:A15" si="3">$B$1^2*4*B6/(9)</f>
-        <v>6.8376068376068387E-6</v>
+        <v>6.8376068376068378E-7</v>
       </c>
       <c r="B6">
-        <f>1000*10^-6</f>
-        <v>1E-3</v>
+        <f>100*10^-6</f>
+        <v>9.9999999999999991E-5</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>750</v>
+        <v>15000.000000000002</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>4.9606400825913009E-4</v>
+        <v>4.9606400825913007E-5</v>
       </c>
       <c r="H6">
-        <f>1000*10^-6</f>
-        <v>1E-3</v>
+        <f>100*10^-6</f>
+        <v>9.9999999999999991E-5</v>
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>48.387096774193552</v>
+        <v>967.74193548387098</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="3"/>
-        <v>1.5042735042735044E-7</v>
+        <v>3.213675213675214E-6</v>
       </c>
       <c r="B7">
-        <f>22*10^-6</f>
-        <v>2.1999999999999999E-5</v>
+        <f>470*10^-6</f>
+        <v>4.6999999999999999E-4</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>34090.909090909088</v>
+        <v>3191.4893617021276</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1.0913408181700861E-5</v>
+        <v>2.3315008388179114E-4</v>
       </c>
       <c r="H7">
-        <f>22*10^-6</f>
-        <v>2.1999999999999999E-5</v>
+        <f>470*10^-6</f>
+        <v>4.6999999999999999E-4</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>2199.4134897360705</v>
+        <v>205.90253946465342</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="3"/>
-        <v>3.2136752136752138E-7</v>
-      </c>
-      <c r="B8">
-        <f>47*10^-6</f>
-        <v>4.6999999999999997E-5</v>
-      </c>
-      <c r="C8">
+      <c r="A8" s="1">
+        <f t="shared" si="3"/>
+        <v>6.8376068376068387E-6</v>
+      </c>
+      <c r="B8" s="1">
+        <f>1000*10^-6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>15957.44680851064</v>
+        <v>1500</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" t="e">
+        <v>4.9606400825913009E-4</v>
+      </c>
+      <c r="H8">
+        <f>1000*10^-6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>96.774193548387103</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C9" t="e">
+        <v>6.8376068376068387E-6</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B15" si="4">1000*10^-6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1500</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" t="e">
+        <v>4.9606400825913009E-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H15" si="5">1000*10^-6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>96.774193548387103</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C10" t="e">
+        <v>6.8376068376068387E-6</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="4"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1500</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" t="e">
+        <v>4.9606400825913009E-4</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>96.774193548387103</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C11" t="e">
+        <v>6.8376068376068387E-6</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="4"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" t="e">
+        <v>1500</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>96.774193548387103</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C12" t="e">
+        <v>6.8376068376068387E-6</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="4"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C12">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1500</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>96.774193548387103</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C13" t="e">
+        <v>6.8376068376068387E-6</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="4"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1500</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>96.774193548387103</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C14" t="e">
+        <v>6.8376068376068387E-6</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="4"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1500</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>96.774193548387103</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C15" t="e">
+        <v>6.8376068376068387E-6</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="4"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1500</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>96.774193548387103</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1573,6 +1564,9 @@
       <c r="G23" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H23" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1591,6 +1585,10 @@
         <f>G22*4</f>
         <v>0.57607433217189308</v>
       </c>
+      <c r="H24">
+        <f>G24/2</f>
+        <v>0.28803716608594654</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Informe final 04 - previo 05
</commit_message>
<xml_diff>
--- a/4. CONTROLADOR PID/INFORME PREVIO/calculo_rc.xlsx
+++ b/4. CONTROLADOR PID/INFORME PREVIO/calculo_rc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\lab-control-i\4. CONTROLADOR PID\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0AE6A8-0830-4B6A-BB2D-00574307F44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E866B03-8871-4F46-BB4A-2FC5250E2B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="13935" windowHeight="16200" activeTab="1" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
+    <workbookView xWindow="14865" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815D4429-F3D6-4F7B-A018-34B483DED09C}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03516E6C-2C46-4AD1-BC3F-907E935C7AD3}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
COMPENSADOR PD - PID - analisis a lazo abierto
</commit_message>
<xml_diff>
--- a/4. CONTROLADOR PID/INFORME PREVIO/calculo_rc.xlsx
+++ b/4. CONTROLADOR PID/INFORME PREVIO/calculo_rc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\lab-control-i\4. CONTROLADOR PID\INFORME PREVIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\lab-control-i\4. CONTROLADOR PID\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E866B03-8871-4F46-BB4A-2FC5250E2B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92970A4-0A97-4072-A1EB-544BDB4E36E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
+    <workbookView xWindow="72" yWindow="1092" windowWidth="11508" windowHeight="11580" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
   <si>
     <t>R</t>
   </si>
@@ -494,18 +494,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815D4429-F3D6-4F7B-A018-34B483DED09C}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -517,7 +517,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -545,7 +545,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>$B$2^2*4*B4/(9)</f>
         <v>1.3675213675213676E-6</v>
@@ -591,7 +591,7 @@
         <v>7142.8571428571431</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>$B$2^2*4*B5/(9)</f>
         <v>6.427350427350428E-6</v>
@@ -617,7 +617,7 @@
         <v>1519.7568389057751</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>$B$2^2*4*B6/(9)</f>
         <v>1.3675213675213674E-5</v>
@@ -643,7 +643,7 @@
         <v>714.28571428571433</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" ref="A7:A16" si="3">$B$2^2*4*B7/(9)</f>
         <v>6.4273504273504274E-5</v>
@@ -669,7 +669,7 @@
         <v>151.9756838905775</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
@@ -695,7 +695,7 @@
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>3.0085470085470087E-6</v>
@@ -721,7 +721,7 @@
         <v>3246.7532467532469</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
@@ -747,7 +747,7 @@
         <v>15197.568389057751</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
@@ -761,7 +761,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
@@ -775,7 +775,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
@@ -789,7 +789,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
@@ -803,7 +803,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
@@ -817,7 +817,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
@@ -831,10 +831,10 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -848,7 +848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>325</v>
       </c>
@@ -864,7 +864,7 @@
         <v>20.994046775217015</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
@@ -872,7 +872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23">
         <f>D2/(2*B21)</f>
         <v>0.55470019622522915</v>
@@ -882,7 +882,7 @@
         <v>1.000283567282036</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F25" s="1" t="s">
         <v>13</v>
       </c>
@@ -890,7 +890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F26">
         <f>(2*G23)/G21</f>
         <v>9.5292115711854808E-2</v>
@@ -900,13 +900,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="F27" s="1" t="s">
         <v>21</v>
       </c>
@@ -914,7 +912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -930,7 +928,7 @@
         <v>0.19058423142370962</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>325</v>
       </c>
@@ -939,18 +937,18 @@
         <v>18.027756377319946</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31">
         <f>D2/(2*B29)</f>
         <v>0.55470019622522915</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -958,7 +956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <f>PI()/(B33)</f>
         <v>0.20943951023931953</v>
@@ -968,7 +966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -976,7 +974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>4/(B31*B29)</f>
         <v>0.4</v>
@@ -986,7 +984,7 @@
         <v>9.9846035320541246E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -994,7 +992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <f>B29*B31</f>
         <v>10</v>
@@ -1007,7 +1005,7 @@
         <v>6.1805000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -1015,7 +1013,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>1+1*B37%</f>
         <v>1.12361</v>
@@ -1025,7 +1023,7 @@
         <v>1.0618050000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1033,29 +1031,29 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B48" s="3"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
     </row>
@@ -1078,13 +1076,13 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1112,7 +1110,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>$B$1^2*4*B3/(9)</f>
         <v>6.8376068376068386E-8</v>
@@ -1158,7 +1156,7 @@
         <v>9677.419354838712</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>$B$1^2*4*B4/(9)</f>
         <v>1.5042735042735044E-7</v>
@@ -1184,7 +1182,7 @@
         <v>4398.8269794721409</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>$B$1^2*4*B5/(9)</f>
         <v>3.2136752136752138E-7</v>
@@ -1210,7 +1208,7 @@
         <v>2059.0253946465341</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" ref="A6:A15" si="3">$B$1^2*4*B6/(9)</f>
         <v>6.8376068376068378E-7</v>
@@ -1236,7 +1234,7 @@
         <v>967.74193548387098</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="3"/>
         <v>3.213675213675214E-6</v>
@@ -1262,7 +1260,7 @@
         <v>205.90253946465342</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>6.8376068376068387E-6</v>
@@ -1288,7 +1286,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>6.8376068376068387E-6</v>
@@ -1314,7 +1312,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>6.8376068376068387E-6</v>
@@ -1340,7 +1338,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>6.8376068376068387E-6</v>
@@ -1362,7 +1360,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>6.8376068376068387E-6</v>
@@ -1384,7 +1382,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>6.8376068376068387E-6</v>
@@ -1406,7 +1404,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>6.8376068376068387E-6</v>
@@ -1428,7 +1426,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>6.8376068376068387E-6</v>
@@ -1450,7 +1448,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1461,7 +1459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1481,7 +1479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>65</v>
       </c>
@@ -1505,7 +1503,7 @@
         <v>1.0564771737160452</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1525,7 +1523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <f>B20*SQRT(1-C20^2)</f>
         <v>7.9999999999999991</v>
@@ -1551,7 +1549,7 @@
         <v>15.499999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -1568,7 +1566,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <f>4/(C20*B20)</f>
         <v>4</v>

</xml_diff>